<commit_message>
update code show page server
</commit_message>
<xml_diff>
--- a/limpios.xlsx
+++ b/limpios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V105"/>
+  <dimension ref="A1:U105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,12 +536,7 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>correo</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>correo.1</t>
+          <t>company_email</t>
         </is>
       </c>
     </row>
@@ -607,7 +602,6 @@
           <t>info@theaestheticsdoctor.com, mike.rushton@stackwizards.com, jack@gibsonhaus.com, alistair.hey@stackwizards.com, james@gibsonhaus.com, media.bobbledigital@gmail.com</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -643,7 +637,6 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -726,10 +719,9 @@
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr">
         <is>
-          <t>info@lmaclinic.com, wixodday@wix.com</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr"/>
+          <t>info@lmaclinic.com</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -809,7 +801,6 @@
           <t>houston@sisuclinic.com, fortlauderdale@sisuclinic.com, soho@sisuclinic.com, flatiron@sisuclinic.com, brickell@sisuclinic.com, merrick@sisuclinic.com, info@sisuclinic.com, pat@sisuclinic.com, press@sisuclinic.com</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -841,7 +832,6 @@
       <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -880,10 +870,9 @@
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr">
         <is>
-          <t>asdsd@wix.com, info@mcliniclondon.co.uk</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr"/>
+          <t>info@mcliniclondon.co.uk</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -939,7 +928,6 @@
           <t>hello@drwellsaesthetics.com, hello@drwellsclinic.co.uk</t>
         </is>
       </c>
-      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1017,7 +1005,6 @@
           <t>reception@drgabriela.co.uk</t>
         </is>
       </c>
-      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1049,7 +1036,6 @@
       <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1085,7 +1071,6 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1121,7 +1106,6 @@
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1193,7 +1177,6 @@
           <t>london@picoclinics.com, milan@picoclinics.com, losangeles@picoclinics.com, newyork@picoclinics.com</t>
         </is>
       </c>
-      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1241,7 +1224,6 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1277,7 +1259,6 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1349,7 +1330,6 @@
           <t>contact@domain.co.uk</t>
         </is>
       </c>
-      <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1413,7 +1393,6 @@
           <t>enquiries@harleystreetskinclinic.com</t>
         </is>
       </c>
-      <c r="V17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1481,7 +1460,6 @@
           <t>info@thelondoncosmeticclinic.co.uk</t>
         </is>
       </c>
-      <c r="V18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1551,7 +1529,6 @@
           <t>team@antiwrinkleclinic.co.uk, affiliates@antiwrinkleclinic.co.uk</t>
         </is>
       </c>
-      <c r="V19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1623,7 +1600,6 @@
           <t>bookings@regentsparkaesthetics.co.uk</t>
         </is>
       </c>
-      <c r="V20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1687,7 +1663,6 @@
           <t>info@londonaestheticsclinic.co.uk</t>
         </is>
       </c>
-      <c r="V21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1760,7 +1735,6 @@
           <t>info@aestha.co.uk</t>
         </is>
       </c>
-      <c r="V22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1792,7 +1766,6 @@
       <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1828,7 +1801,6 @@
       <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1864,7 +1836,6 @@
       <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1896,7 +1867,6 @@
       <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1960,7 +1930,6 @@
           <t>info@london-aesthetic-medicine.com</t>
         </is>
       </c>
-      <c r="V27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2032,7 +2001,6 @@
           <t>info@asthetiklondon.com</t>
         </is>
       </c>
-      <c r="V28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2064,7 +2032,6 @@
       <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2100,7 +2067,6 @@
       <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2164,7 +2130,6 @@
           <t>contact@drfillerlondon.com</t>
         </is>
       </c>
-      <c r="V31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2208,7 +2173,6 @@
           <t>chenowith52@gmail.com, test@test.com, test@gmail.com, test@mail.com</t>
         </is>
       </c>
-      <c r="V32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2272,7 +2236,6 @@
           <t>enquiry@vaaesthetics.com</t>
         </is>
       </c>
-      <c r="V33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2332,7 +2295,6 @@
       <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2372,7 +2334,6 @@
       <c r="S35" t="inlineStr"/>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
-      <c r="V35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2452,7 +2413,6 @@
           <t>london@ouronyx.com, dubai@ouronyx.com</t>
         </is>
       </c>
-      <c r="V36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2488,7 +2448,6 @@
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2544,7 +2503,6 @@
           <t>info@drdray.co.uk</t>
         </is>
       </c>
-      <c r="V38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2594,7 +2552,6 @@
           <t>info@doctorvoss.com</t>
         </is>
       </c>
-      <c r="V39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2658,7 +2615,6 @@
           <t>enquiry@vaaesthetics.com</t>
         </is>
       </c>
-      <c r="V40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2728,7 +2684,6 @@
           <t>ighanem@doctors.net.uk, contact@drinjyghanem.co.uk</t>
         </is>
       </c>
-      <c r="V41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2814,7 +2769,6 @@
           <t>info@clinicbe.com</t>
         </is>
       </c>
-      <c r="V42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2850,7 +2804,6 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2882,7 +2835,6 @@
       <c r="S44" t="inlineStr"/>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
-      <c r="V44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2942,7 +2894,6 @@
           <t>info@aesthetic-clinics.co.uk, info@aesthetic-clinic.co.uk, info@drglancey-clinics.com</t>
         </is>
       </c>
-      <c r="V45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3006,7 +2957,6 @@
           <t>info@avicennawellbeing.com</t>
         </is>
       </c>
-      <c r="V46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3077,7 +3027,6 @@
           <t>info@amsaesthetics.com</t>
         </is>
       </c>
-      <c r="V47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3129,7 +3078,6 @@
           <t>contact@atyu.co.uk</t>
         </is>
       </c>
-      <c r="V48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3165,7 +3113,6 @@
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
-      <c r="V49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3245,7 +3192,6 @@
           <t>info@oneskinclinic.co.uk</t>
         </is>
       </c>
-      <c r="V50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3317,7 +3263,6 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
-      <c r="V51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3349,7 +3294,6 @@
       <c r="S52" t="inlineStr"/>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
-      <c r="V52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3381,7 +3325,6 @@
       <c r="S53" t="inlineStr"/>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
-      <c r="V53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3445,7 +3388,6 @@
           <t>spa@essentialslondon.com</t>
         </is>
       </c>
-      <c r="V54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3481,7 +3423,6 @@
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
-      <c r="V55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3565,7 +3506,6 @@
           <t>cadogan@cadoganclinic.com</t>
         </is>
       </c>
-      <c r="V56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3621,7 +3561,6 @@
           <t>info@dmcaesthetics.com</t>
         </is>
       </c>
-      <c r="V57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3697,7 +3636,6 @@
           <t>drhotaki@hotaki.co.uk</t>
         </is>
       </c>
-      <c r="V58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3757,7 +3695,6 @@
       <c r="S59" t="inlineStr"/>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
-      <c r="V59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3825,7 +3762,6 @@
           <t>hello@juicyface.co.uk</t>
         </is>
       </c>
-      <c r="V60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3893,7 +3829,6 @@
           <t>info@pulse-clinic.co.uk, info@pulseclinic.co.uk</t>
         </is>
       </c>
-      <c r="V61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3969,7 +3904,6 @@
       <c r="S62" t="inlineStr"/>
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr"/>
-      <c r="V62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4035,7 +3969,6 @@
       <c r="S63" t="inlineStr"/>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
-      <c r="V63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4067,7 +4000,6 @@
       <c r="S64" t="inlineStr"/>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
-      <c r="V64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4139,7 +4071,6 @@
           <t>info@drjoneydesouza.com</t>
         </is>
       </c>
-      <c r="V65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4211,7 +4142,6 @@
           <t>info@waterhouseyoung.com</t>
         </is>
       </c>
-      <c r="V66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -4247,7 +4177,6 @@
       <c r="S67" t="inlineStr"/>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
-      <c r="V67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -4283,7 +4212,6 @@
       <c r="S68" t="inlineStr"/>
       <c r="T68" t="inlineStr"/>
       <c r="U68" t="inlineStr"/>
-      <c r="V68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -4315,7 +4243,6 @@
       <c r="S69" t="inlineStr"/>
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
-      <c r="V69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -4351,7 +4278,6 @@
       <c r="S70" t="inlineStr"/>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
-      <c r="V70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -4395,7 +4321,6 @@
           <t>info@bea-skin.com</t>
         </is>
       </c>
-      <c r="V71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4431,7 +4356,6 @@
       <c r="S72" t="inlineStr"/>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
-      <c r="V72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4503,7 +4427,6 @@
           <t>pr@drdandhunna.com</t>
         </is>
       </c>
-      <c r="V73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4571,7 +4494,6 @@
       <c r="S74" t="inlineStr"/>
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
-      <c r="V74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4631,7 +4553,6 @@
           <t>hello@omniya.co.uk</t>
         </is>
       </c>
-      <c r="V75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4667,7 +4588,6 @@
       <c r="S76" t="inlineStr"/>
       <c r="T76" t="inlineStr"/>
       <c r="U76" t="inlineStr"/>
-      <c r="V76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4747,7 +4667,6 @@
           <t>enquiries@cosmedics.co.uk</t>
         </is>
       </c>
-      <c r="V77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4819,7 +4738,6 @@
           <t>mail@mayfairpractice.com</t>
         </is>
       </c>
-      <c r="V78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4890,7 +4808,6 @@
           <t>hello@dermacureclinic.co.uk</t>
         </is>
       </c>
-      <c r="V79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4926,7 +4843,6 @@
       <c r="S80" t="inlineStr"/>
       <c r="T80" t="inlineStr"/>
       <c r="U80" t="inlineStr"/>
-      <c r="V80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4990,7 +4906,6 @@
       <c r="S81" t="inlineStr"/>
       <c r="T81" t="inlineStr"/>
       <c r="U81" t="inlineStr"/>
-      <c r="V81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -5022,7 +4937,6 @@
       <c r="S82" t="inlineStr"/>
       <c r="T82" t="inlineStr"/>
       <c r="U82" t="inlineStr"/>
-      <c r="V82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -5070,7 +4984,6 @@
           <t>info@uskinclinic.com</t>
         </is>
       </c>
-      <c r="V83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -5150,7 +5063,6 @@
           <t>reception@facecliniclondon.com</t>
         </is>
       </c>
-      <c r="V84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -5222,7 +5134,6 @@
           <t>info@wimpoleaesthetics.co.uk</t>
         </is>
       </c>
-      <c r="V85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -5306,7 +5217,6 @@
       <c r="S86" t="inlineStr"/>
       <c r="T86" t="inlineStr"/>
       <c r="U86" t="inlineStr"/>
-      <c r="V86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -5378,7 +5288,6 @@
       <c r="S87" t="inlineStr"/>
       <c r="T87" t="inlineStr"/>
       <c r="U87" t="inlineStr"/>
-      <c r="V87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -5438,7 +5347,6 @@
           <t>info@skinscienceclinic.co.uk</t>
         </is>
       </c>
-      <c r="V88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -5510,7 +5418,6 @@
       <c r="S89" t="inlineStr"/>
       <c r="T89" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
-      <c r="V89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -5568,7 +5475,6 @@
           <t>info@sloaneclinic.co.uk</t>
         </is>
       </c>
-      <c r="V90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5600,7 +5506,6 @@
       <c r="S91" t="inlineStr"/>
       <c r="T91" t="inlineStr"/>
       <c r="U91" t="inlineStr"/>
-      <c r="V91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5664,7 +5569,6 @@
           <t>paul@searchvista.co.uk</t>
         </is>
       </c>
-      <c r="V92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5724,7 +5628,6 @@
           <t>laclinicsuk@gmail.com, info@laclinicsuk.com</t>
         </is>
       </c>
-      <c r="V93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5788,7 +5691,6 @@
           <t>info@shapeandtoneaesthetics.com</t>
         </is>
       </c>
-      <c r="V94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5852,7 +5754,6 @@
           <t>clinics@dermamedical.co.uk</t>
         </is>
       </c>
-      <c r="V95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5908,7 +5809,6 @@
       <c r="S96" t="inlineStr"/>
       <c r="T96" t="inlineStr"/>
       <c r="U96" t="inlineStr"/>
-      <c r="V96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5940,7 +5840,6 @@
       <c r="S97" t="inlineStr"/>
       <c r="T97" t="inlineStr"/>
       <c r="U97" t="inlineStr"/>
-      <c r="V97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5976,7 +5875,6 @@
       <c r="S98" t="inlineStr"/>
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
-      <c r="V98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -6008,7 +5906,6 @@
       <c r="S99" t="inlineStr"/>
       <c r="T99" t="inlineStr"/>
       <c r="U99" t="inlineStr"/>
-      <c r="V99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -6072,7 +5969,6 @@
           <t>firstaesthetics@outlook.com</t>
         </is>
       </c>
-      <c r="V100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -6140,7 +6036,6 @@
           <t>filler@godaddy.com</t>
         </is>
       </c>
-      <c r="V101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -6224,7 +6119,6 @@
       <c r="S102" t="inlineStr"/>
       <c r="T102" t="inlineStr"/>
       <c r="U102" t="inlineStr"/>
-      <c r="V102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -6308,7 +6202,6 @@
       <c r="S103" t="inlineStr"/>
       <c r="T103" t="inlineStr"/>
       <c r="U103" t="inlineStr"/>
-      <c r="V103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -6340,7 +6233,6 @@
       <c r="S104" t="inlineStr"/>
       <c r="T104" t="inlineStr"/>
       <c r="U104" t="inlineStr"/>
-      <c r="V104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -6424,7 +6316,6 @@
       <c r="S105" t="inlineStr"/>
       <c r="T105" t="inlineStr"/>
       <c r="U105" t="inlineStr"/>
-      <c r="V105" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>